<commit_message>
handle empty field, array data
</commit_message>
<xml_diff>
--- a/data/sample-1.xlsx
+++ b/data/sample-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <r>
       <t>a</t>
@@ -239,6 +239,26 @@
   </si>
   <si>
     <t>sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>empty_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>["a", "b", "c"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -627,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -776,6 +796,28 @@
         <v>33</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>